<commit_message>
idk need to review
</commit_message>
<xml_diff>
--- a/SAMPLE.xlsx
+++ b/SAMPLE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Desktop/MAPS_proj/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CAT_proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D45EFF-2058-DA4D-BB61-BE23858674D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A90DCBC-D582-4063-9CC2-C0EA12793C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="עיקור חתולים" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="305">
   <si>
     <t>(אל תשנה) פנייה</t>
   </si>
@@ -637,13 +637,324 @@
   </si>
   <si>
     <t>כתובת תחילה</t>
+  </si>
+  <si>
+    <t>אריאלה אריאלה</t>
+  </si>
+  <si>
+    <t>אור יהודה</t>
+  </si>
+  <si>
+    <t>החצב</t>
+  </si>
+  <si>
+    <t>0527001358</t>
+  </si>
+  <si>
+    <t>מבקשת עיקור וסירוס של חתולי חצר.  מאכילה בוקר וערב אך אין שעות האכלה</t>
+  </si>
+  <si>
+    <t>אין שעות מסוימות</t>
+  </si>
+  <si>
+    <t>14645-2023</t>
+  </si>
+  <si>
+    <t>קליינמן דניאלה</t>
+  </si>
+  <si>
+    <t>גן חיים</t>
+  </si>
+  <si>
+    <t>דרך המלך</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>0547380315</t>
+  </si>
+  <si>
+    <t>עיקור חתולה צבע שחור לבן עם , פנים שחורות וסימן לבן על החזה , כבר ילדה 10 גורים , מבקשת סירוס דחוף</t>
+  </si>
+  <si>
+    <t>00:00</t>
+  </si>
+  <si>
+    <t>14464-2023</t>
+  </si>
+  <si>
+    <t>לוז ציונה</t>
+  </si>
+  <si>
+    <t>ירקונה</t>
+  </si>
+  <si>
+    <t>050-6878490</t>
+  </si>
+  <si>
+    <t>בבקשה לחזור טלפונית לתושבת- מעוניינת לקבל מידע בנוגע לשירותים וטרינריים לגבי חתולים</t>
+  </si>
+  <si>
+    <t>11896-2023</t>
+  </si>
+  <si>
+    <t>בלס רינה</t>
+  </si>
+  <si>
+    <t>הרצל</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>035332758</t>
+  </si>
+  <si>
+    <t>20.8 אין מענה מבקשת לעקר חתולה גדולה (לא יודעת צבעים) - שמגיעה כל ערב לגורים שלה - כי היא ממליטה כל כמה חודשים.&lt;br /&gt;
+מבקשת לקחת את הגורים משם כי הם מפריעים לה.
+מרגלית - חתולה אחת לעיקור בערב.  מאוד דחוף</t>
+  </si>
+  <si>
+    <t>ערב.  אין שעות מסוימות</t>
+  </si>
+  <si>
+    <t>11454-2023</t>
+  </si>
+  <si>
+    <t>הלחמי עידית</t>
+  </si>
+  <si>
+    <t>ירחיב</t>
+  </si>
+  <si>
+    <t>אנפה</t>
+  </si>
+  <si>
+    <t>0525536464</t>
+  </si>
+  <si>
+    <t>20:00 15</t>
+  </si>
+  <si>
+    <t>יעקובי שחר</t>
+  </si>
+  <si>
+    <t>שחר יעקובי</t>
+  </si>
+  <si>
+    <t>11110-2023</t>
+  </si>
+  <si>
+    <t>סרוסי איציק</t>
+  </si>
+  <si>
+    <t>אלישמע</t>
+  </si>
+  <si>
+    <t>הנרקיס</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>0503500350</t>
+  </si>
+  <si>
+    <t>עיקור עיקור חתולים רחוב</t>
+  </si>
+  <si>
+    <t>09:30</t>
+  </si>
+  <si>
+    <t>10642-2023</t>
+  </si>
+  <si>
+    <t>חמלניצקי קטיה</t>
+  </si>
+  <si>
+    <t>שד בגין מנחם</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>0509338553</t>
+  </si>
+  <si>
+    <t>9.7 מוכנה להקדים את שעת ההאכלה באופן הדרגתי ל22:00</t>
+  </si>
+  <si>
+    <t>10200-2023</t>
+  </si>
+  <si>
+    <t>אלמגור דקלה</t>
+  </si>
+  <si>
+    <t>שדה ורבורג</t>
+  </si>
+  <si>
+    <t>0509717615</t>
+  </si>
+  <si>
+    <t>====קיימת כבר פניה 8046 מיום 31.5=======
+מבקשים בהקדם עיקור/סירוס אומרים כי המצב בלתי נסבל</t>
+  </si>
+  <si>
+    <t>07.00</t>
+  </si>
+  <si>
+    <t>10049-2023</t>
+  </si>
+  <si>
+    <t>גנדליס חן</t>
+  </si>
+  <si>
+    <t>גני תקווה</t>
+  </si>
+  <si>
+    <t>הרי יהודה</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>0508439259</t>
+  </si>
+  <si>
+    <t>16.8 תהיה בחו"ל רלוונטי מה26.8 8.8 נסיון תיאום 16.7 1 +1 מזדמן, עודכנו שעות וימים ומבררת מי עוד מאכיל דרך אריאל . 27.6 לא פנויה עיקור עיקור חתולה שככל הנראה כבר בהריון וחתול נוסף לסירוס</t>
+  </si>
+  <si>
+    <t>18:30-19:00 יום א +ה</t>
+  </si>
+  <si>
+    <t>9450-2023</t>
+  </si>
+  <si>
+    <t>דורון יונה</t>
+  </si>
+  <si>
+    <t>כפר מעש</t>
+  </si>
+  <si>
+    <t>הצבעוני</t>
+  </si>
+  <si>
+    <t>הצבעוני 6</t>
+  </si>
+  <si>
+    <t>0549911204</t>
+  </si>
+  <si>
+    <t>3.4 אין מענה עיקור הגיעה לחצר שלנו חתולה חדשה שכנראה אינה מעוקרת.מבקשת ללכוד ולעקר.שעות האכלה של החתולים הן 6:30-7:00 בבוקר וגם אחהצ</t>
+  </si>
+  <si>
+    <t>06:30-7:00, 16:00</t>
+  </si>
+  <si>
+    <t>4214-2023</t>
+  </si>
+  <si>
+    <t>ד"ר צרויה יאיר</t>
+  </si>
+  <si>
+    <t>09-7707111</t>
+  </si>
+  <si>
+    <t>מאכיל חתולים.  שעות האכלה ערב.  אין שעות מסוימות.  כ-5 חתולים.  נמצאים ליד הבית הפנימי במגרש</t>
+  </si>
+  <si>
+    <t>245-2022</t>
+  </si>
+  <si>
+    <t>קראדי יוהנה</t>
+  </si>
+  <si>
+    <t>עדנים</t>
+  </si>
+  <si>
+    <t>הרקון</t>
+  </si>
+  <si>
+    <t>0544213484</t>
+  </si>
+  <si>
+    <t>עיקור/סירוס 2 חתולים מעונינת להביא עצמאית. היא לא המאכילה</t>
+  </si>
+  <si>
+    <t>10677-2023</t>
+  </si>
+  <si>
+    <t>רצון צופית</t>
+  </si>
+  <si>
+    <t>קורצ'ק</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>054-4477995</t>
+  </si>
+  <si>
+    <t>18:00 1</t>
+  </si>
+  <si>
+    <t>מוכתר אור</t>
+  </si>
+  <si>
+    <t>אור</t>
+  </si>
+  <si>
+    <t>10626-2023</t>
+  </si>
+  <si>
+    <t>0 חן</t>
+  </si>
+  <si>
+    <t>הרא"ה</t>
+  </si>
+  <si>
+    <t>119</t>
+  </si>
+  <si>
+    <t>052-4787792</t>
+  </si>
+  <si>
+    <t>מרגלית.  החתול, לדברי הפונה, הוא מאוד תוקפני.  תוקף את כולם.  מפחדת לרדת במדרגות.  לא זזה משם.  דחוף מאוד.  לא מאכילה
+חתולה תוקפנית מתחת לבית תוקפת אנשים וגם כלבים חתולה עם פסים חום שחור ואפור לא בורחת שמתקרבים אליה חושפת שיניים נראת בריאה מסתובבת ליד האטליז בחיבת ציון פינת הרואה , הגיעה בשבוע שעבר פקח והסביר איך להרחיק אותה אלה שהחתול שוב חזר וסרט את הכלבה של הפונה מבקש שיקחו אותה או שיפנו אותה דחוף מהמקום</t>
+  </si>
+  <si>
+    <t>10596-2023</t>
+  </si>
+  <si>
+    <t>שלב הדס</t>
+  </si>
+  <si>
+    <t>גבעת שמואל</t>
+  </si>
+  <si>
+    <t>הנשיא</t>
+  </si>
+  <si>
+    <t>21 ד'</t>
+  </si>
+  <si>
+    <t>0547380272</t>
+  </si>
+  <si>
+    <t>מדווחת על כ-30 חתולים שיש ברחוב בכתובת.  מבקשת עיקור/סירוס
+לא מאכילה</t>
+  </si>
+  <si>
+    <t>10509-2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
@@ -657,6 +968,18 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -705,7 +1028,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -713,6 +1036,30 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -759,9 +1106,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -799,7 +1146,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -905,7 +1252,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1047,7 +1394,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1056,13 +1403,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="dataSheet"/>
-  <dimension ref="A1:S23"/>
+  <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="D1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="D16" zoomScale="117" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="0" style="1" hidden="1" customWidth="1"/>
@@ -1074,7 +1421,7 @@
     <col min="14" max="19" width="28" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1133,7 +1480,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1180,7 +1527,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1221,7 +1568,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -1262,7 +1609,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -1303,7 +1650,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -1344,7 +1691,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>65</v>
       </c>
@@ -1388,7 +1735,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>73</v>
       </c>
@@ -1435,7 +1782,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>81</v>
       </c>
@@ -1476,7 +1823,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>89</v>
       </c>
@@ -1523,7 +1870,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>96</v>
       </c>
@@ -1573,7 +1920,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>105</v>
       </c>
@@ -1623,7 +1970,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>115</v>
       </c>
@@ -1667,7 +2014,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>123</v>
       </c>
@@ -1717,7 +2064,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>133</v>
       </c>
@@ -1758,7 +2105,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>138</v>
       </c>
@@ -1799,7 +2146,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>147</v>
       </c>
@@ -1834,7 +2181,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>153</v>
       </c>
@@ -1878,7 +2225,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>160</v>
       </c>
@@ -1925,7 +2272,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>166</v>
       </c>
@@ -1972,7 +2319,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>173</v>
       </c>
@@ -2010,7 +2357,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>180</v>
       </c>
@@ -2060,7 +2407,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>189</v>
       </c>
@@ -2102,6 +2449,642 @@
       </c>
       <c r="S23" s="1" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D24" s="7">
+        <v>45221.380219907405</v>
+      </c>
+      <c r="E24"/>
+      <c r="F24" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="K24" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="L24" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="M24" s="10">
+        <v>5</v>
+      </c>
+      <c r="N24" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="O24"/>
+      <c r="P24"/>
+      <c r="Q24" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="R24" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S24" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D25" s="7">
+        <v>45215.777349537035</v>
+      </c>
+      <c r="E25"/>
+      <c r="F25" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="K25" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="L25" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="M25" s="10">
+        <v>1</v>
+      </c>
+      <c r="N25" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="O25"/>
+      <c r="P25"/>
+      <c r="Q25" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="R25" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S25" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D26" s="7">
+        <v>45152.479826388888</v>
+      </c>
+      <c r="E26"/>
+      <c r="F26" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="L26" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="M26" s="10">
+        <v>1</v>
+      </c>
+      <c r="N26" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="O26"/>
+      <c r="P26"/>
+      <c r="Q26" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="R26" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S26" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D27" s="7">
+        <v>45142.51840277778</v>
+      </c>
+      <c r="E27"/>
+      <c r="F27" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="J27" s="11"/>
+      <c r="K27" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="L27" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="M27" s="10">
+        <v>1</v>
+      </c>
+      <c r="N27" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="O27"/>
+      <c r="P27"/>
+      <c r="Q27" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="R27" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S27" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D28" s="7">
+        <v>45133.532326388886</v>
+      </c>
+      <c r="E28"/>
+      <c r="F28" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="I28" s="12"/>
+      <c r="J28" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="K28" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="L28" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="M28" s="10">
+        <v>5</v>
+      </c>
+      <c r="N28" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="O28" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="P28" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q28" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="R28" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="S28" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D29" s="7">
+        <v>45123.663495370369</v>
+      </c>
+      <c r="E29"/>
+      <c r="F29" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="K29" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="L29" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="M29" s="10">
+        <v>8</v>
+      </c>
+      <c r="N29" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="O29"/>
+      <c r="P29"/>
+      <c r="Q29" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="R29" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S29" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D30" s="7">
+        <v>45115.572835648149</v>
+      </c>
+      <c r="E30"/>
+      <c r="F30" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="J30" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="K30" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="L30" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="M30" s="10">
+        <v>10</v>
+      </c>
+      <c r="N30" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="O30"/>
+      <c r="P30"/>
+      <c r="Q30" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="R30" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="S30" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D31" s="7">
+        <v>45112.502141203702</v>
+      </c>
+      <c r="E31"/>
+      <c r="F31" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="H31" s="11"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="L31" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="M31" s="10">
+        <v>10</v>
+      </c>
+      <c r="N31" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="O31"/>
+      <c r="P31"/>
+      <c r="Q31" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="R31" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S31" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D32" s="7">
+        <v>45103.442037037035</v>
+      </c>
+      <c r="E32"/>
+      <c r="F32" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="J32" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="K32" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="L32" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="M32" s="10">
+        <v>1</v>
+      </c>
+      <c r="N32" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="O32"/>
+      <c r="P32"/>
+      <c r="Q32" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="R32" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S32" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="D33" s="7">
+        <v>45006.289421296293</v>
+      </c>
+      <c r="E33"/>
+      <c r="F33" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="J33" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="K33" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="L33" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="M33" s="10">
+        <v>1</v>
+      </c>
+      <c r="N33" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="O33"/>
+      <c r="P33"/>
+      <c r="Q33" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="R33" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S33" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="D34" s="7">
+        <v>44567.66300925926</v>
+      </c>
+      <c r="E34"/>
+      <c r="F34" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="J34" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="K34" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="L34" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="M34" s="10">
+        <v>5</v>
+      </c>
+      <c r="N34" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="R34" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S34" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="D35" s="7">
+        <v>45124.401203703703</v>
+      </c>
+      <c r="E35"/>
+      <c r="F35" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I35" s="12"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="L35" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="M35" s="14"/>
+      <c r="N35" s="12"/>
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="R35" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S35" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="D36" s="7">
+        <v>45123.543333333335</v>
+      </c>
+      <c r="E36"/>
+      <c r="F36" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="J36" s="11"/>
+      <c r="K36" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="L36" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="M36" s="14"/>
+      <c r="N36" s="12"/>
+      <c r="O36" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="P36" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="Q36" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="R36" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="S36" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="D37" s="7">
+        <v>45123.335844907408</v>
+      </c>
+      <c r="E37"/>
+      <c r="F37" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="J37" s="11"/>
+      <c r="K37" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="L37" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="M37" s="10">
+        <v>1</v>
+      </c>
+      <c r="N37" s="12"/>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="R37" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S37" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="D38" s="7">
+        <v>45120.395856481482</v>
+      </c>
+      <c r="E38"/>
+      <c r="F38" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="J38" s="11"/>
+      <c r="K38" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="L38" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="M38" s="10">
+        <v>30</v>
+      </c>
+      <c r="N38" s="12"/>
+      <c r="O38"/>
+      <c r="P38"/>
+      <c r="Q38" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="R38" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S38" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2167,9 +3150,9 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>201</v>
       </c>
@@ -2177,7 +3160,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>21</v>
       </c>
@@ -2185,7 +3168,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>32</v>
       </c>
@@ -2193,7 +3176,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>42</v>
       </c>
@@ -2201,7 +3184,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>50</v>
       </c>
@@ -2209,7 +3192,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>58</v>
       </c>
@@ -2217,7 +3200,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>67</v>
       </c>
@@ -2225,7 +3208,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>75</v>
       </c>
@@ -2233,7 +3216,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>83</v>
       </c>
@@ -2241,7 +3224,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>91</v>
       </c>
@@ -2249,7 +3232,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>98</v>
       </c>
@@ -2257,7 +3240,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>107</v>
       </c>
@@ -2265,7 +3248,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>117</v>
       </c>
@@ -2273,7 +3256,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>125</v>
       </c>
@@ -2281,7 +3264,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>125</v>
       </c>
@@ -2289,7 +3272,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>140</v>
       </c>
@@ -2297,7 +3280,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>149</v>
       </c>
@@ -2305,7 +3288,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>155</v>
       </c>
@@ -2329,14 +3312,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>29</v>
       </c>

</xml_diff>